<commit_message>
Final version of OpenAdressing
</commit_message>
<xml_diff>
--- a/aisd_lab_4_hash_table_open_adressing/src/test/java/pl/edu/pw/ee/performance/results/Results.xlsx
+++ b/aisd_lab_4_hash_table_open_adressing/src/test/java/pl/edu/pw/ee/performance/results/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AISD\2021Z_AISD_lab_git_aisd_2021_4_gr21\aisd_lab_4_hash_table_open_adressing\src\test\java\pl\edu\pw\ee\performance\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{738581AD-DBDE-4892-A1EC-1E880B4CE997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A858A90C-D52C-4B17-A77D-AD95848482B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="525" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F731D742-5D35-4953-9DA4-F998327CC1D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F731D742-5D35-4953-9DA4-F998327CC1D4}"/>
   </bookViews>
   <sheets>
     <sheet name="LinearProbing" sheetId="6" r:id="rId1"/>
@@ -6851,7 +6851,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>